<commit_message>
Place and route complete. Silkscreen cleanup needed.
</commit_message>
<xml_diff>
--- a/doc/BOM/AAMB Rev A BOM.xlsx
+++ b/doc/BOM/AAMB Rev A BOM.xlsx
@@ -9,14 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="AAMB." localSheetId="0">Sheet1!$A$1:$H$58</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,21 +23,11 @@
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="AAMB" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\shawn.adams\Documents\Local Files\amp\KiCAD\git\audio_amp_main_board\AAMB." comma="1">
-      <textFields count="2">
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="239">
+  <si>
+    <t>Component Count:</t>
+  </si>
   <si>
     <t>Ref</t>
   </si>
@@ -135,7 +122,7 @@
     <t>Capacitor_SMD:C_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
   </si>
   <si>
-    <t xml:space="preserve">C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, </t>
+    <t xml:space="preserve">C15, C16, C17, C18, C19, C20, C21, C22, C25, C26, C23, C24, </t>
   </si>
   <si>
     <t>0.1u</t>
@@ -147,12 +134,6 @@
     <t>C0603C104Z3VACTU</t>
   </si>
   <si>
-    <t xml:space="preserve">C201, C301, </t>
-  </si>
-  <si>
-    <t>4.7u</t>
-  </si>
-  <si>
     <t xml:space="preserve">C202, C206, C204, C302, C306, C304, </t>
   </si>
   <si>
@@ -249,7 +230,7 @@
     <t>SML-D12U1WT86</t>
   </si>
   <si>
-    <t xml:space="preserve">F1, F2, F4, F3, </t>
+    <t xml:space="preserve">F2, F1, </t>
   </si>
   <si>
     <t>Fuse_Small</t>
@@ -618,45 +599,6 @@
     <t>ERJ-PA3F10R0V</t>
   </si>
   <si>
-    <t xml:space="preserve">TP1, TP2, TP3, TP4, TP5, TP6, </t>
-  </si>
-  <si>
-    <t>TP</t>
-  </si>
-  <si>
-    <t>TestPoint_2Pole</t>
-  </si>
-  <si>
-    <t>TestPoint:TestPoint_2Pads_Pitch2.54mm_Drill0.8mm</t>
-  </si>
-  <si>
-    <t>2-polar test point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP7, TP10, </t>
-  </si>
-  <si>
-    <t>digikey-footprints:Test_Point_D1.02mm</t>
-  </si>
-  <si>
-    <t>PC TEST POINT MINIATURE WHITE</t>
-  </si>
-  <si>
-    <t>Keystone Electronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP8, TP11, </t>
-  </si>
-  <si>
-    <t>PC TEST POINT MINIATURE RED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP9, TP12, </t>
-  </si>
-  <si>
-    <t>PC TEST POINT MINIATURE BLACK</t>
-  </si>
-  <si>
     <t xml:space="preserve">U1, </t>
   </si>
   <si>
@@ -753,12 +695,18 @@
     <t>R_POT</t>
   </si>
   <si>
-    <t>Murata-POT:PV36W202C01B00</t>
+    <t>Potentiometer_THT:Nidec_CT6EP202</t>
   </si>
   <si>
     <t>Potentiometer</t>
   </si>
   <si>
+    <t>Nidec Copal Electronics</t>
+  </si>
+  <si>
+    <t>CT6EP202</t>
+  </si>
+  <si>
     <t xml:space="preserve">VR201, VR301, </t>
   </si>
   <si>
@@ -766,6 +714,33 @@
   </si>
   <si>
     <t>POT-device</t>
+  </si>
+  <si>
+    <t>Potentiometer_THT:Potentiometer_Bourns_3296W_Vertical</t>
+  </si>
+  <si>
+    <t>Bourns Inc.</t>
+  </si>
+  <si>
+    <t>3296W-1-202LF</t>
+  </si>
+  <si>
+    <t>865060640001</t>
+  </si>
+  <si>
+    <t>865080642006</t>
+  </si>
+  <si>
+    <t>885012006053</t>
+  </si>
+  <si>
+    <t>885012006057</t>
+  </si>
+  <si>
+    <t>865080142007</t>
+  </si>
+  <si>
+    <t>865080545012</t>
   </si>
 </sst>
 </file>
@@ -803,14 +778,16 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -823,8 +800,21 @@
 </styleSheet>
 </file>
 
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="AAMB." connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H53" totalsRowShown="0">
+  <autoFilter ref="A1:H53"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Ref"/>
+    <tableColumn id="2" name="Qnty"/>
+    <tableColumn id="3" name="MFG"/>
+    <tableColumn id="4" name="MPN" dataDxfId="0"/>
+    <tableColumn id="5" name="Value"/>
+    <tableColumn id="6" name="Cmp name"/>
+    <tableColumn id="7" name="Footprint"/>
+    <tableColumn id="8" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1090,1497 +1080,1399 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="81.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1">
+        <v>9</v>
+      </c>
+      <c r="B2">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1">
+        <v>16</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
-      </c>
-      <c r="E3">
-        <v>865060640001</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
         <v>20</v>
-      </c>
-      <c r="E4">
-        <v>865080642006</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1">
+        <v>24</v>
+      </c>
+      <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="1">
+        <v>29</v>
+      </c>
+      <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>885012006053</v>
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="1">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8">
-        <v>865080640004</v>
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="1">
-        <v>6</v>
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
         <v>20</v>
-      </c>
-      <c r="E9">
-        <v>885012006057</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
         <v>20</v>
-      </c>
-      <c r="E10">
-        <v>865080142007</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2</v>
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11">
-        <v>865080545012</v>
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="1">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="1">
-        <v>4</v>
+        <v>51</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H13" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="1">
-        <v>11</v>
+        <v>57</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
         <v>54</v>
       </c>
-      <c r="G14" t="s">
-        <v>55</v>
-      </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="1">
+        <v>62</v>
+      </c>
+      <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
+        <v>66</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="1">
+        <v>68</v>
+      </c>
+      <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" t="s">
-        <v>67</v>
+        <v>72</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G16" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="1">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
+        <v>78</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H17" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="1">
-        <v>2</v>
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" t="s">
-        <v>79</v>
+        <v>84</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1935161</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="H19" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="1">
+        <v>91</v>
+      </c>
+      <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20">
-        <v>1935161</v>
+        <v>90</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1935174</v>
+      </c>
+      <c r="E20" t="s">
+        <v>92</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G20" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H20" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="1">
+        <v>95</v>
+      </c>
+      <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21">
-        <v>1935174</v>
+        <v>99</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" t="s">
+        <v>96</v>
       </c>
       <c r="F21" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H21" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="1">
-        <v>2</v>
+        <v>101</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" t="s">
-        <v>100</v>
+        <v>56</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F22" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="G22" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H22" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
       </c>
       <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" t="s">
         <v>103</v>
       </c>
-      <c r="D23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" t="s">
-        <v>104</v>
-      </c>
       <c r="H23" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>107</v>
-      </c>
-      <c r="B24" s="1">
-        <v>6</v>
+        <v>111</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F24" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G24" t="s">
-        <v>104</v>
-      </c>
-      <c r="H24" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25" s="1">
-        <v>2</v>
+        <v>116</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="E25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F25" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" t="s">
         <v>114</v>
       </c>
-      <c r="G25" t="s">
-        <v>115</v>
+      <c r="H25" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="1">
-        <v>5</v>
+        <v>121</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="E26" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F26" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G26" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="H26" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" s="1">
+        <v>127</v>
+      </c>
+      <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="E27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" t="s">
         <v>124</v>
       </c>
-      <c r="G27" t="s">
-        <v>125</v>
-      </c>
       <c r="H27" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="1">
-        <v>2</v>
+        <v>132</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
-      </c>
-      <c r="D28" t="s">
-        <v>57</v>
+        <v>137</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="E28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F28" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="G28" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="H28" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29" s="1">
-        <v>6</v>
+        <v>139</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
       </c>
       <c r="C29" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29">
+        <v>150</v>
+      </c>
+      <c r="F29" t="s">
         <v>134</v>
       </c>
-      <c r="D29" t="s">
-        <v>138</v>
-      </c>
-      <c r="E29" t="s">
-        <v>139</v>
-      </c>
-      <c r="F29" t="s">
-        <v>135</v>
-      </c>
       <c r="G29" t="s">
+        <v>140</v>
+      </c>
+      <c r="H29" t="s">
         <v>136</v>
-      </c>
-      <c r="H29" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>140</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>150</v>
-      </c>
-      <c r="D30" t="s">
-        <v>142</v>
-      </c>
-      <c r="E30" t="s">
         <v>143</v>
       </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30">
+        <v>3.9</v>
+      </c>
       <c r="F30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G30" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31" s="1">
+        <v>147</v>
+      </c>
+      <c r="B31">
         <v>2</v>
       </c>
-      <c r="C31">
-        <v>3.9</v>
-      </c>
-      <c r="D31" t="s">
-        <v>146</v>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F31" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" t="s">
         <v>135</v>
       </c>
-      <c r="G31" t="s">
-        <v>145</v>
-      </c>
       <c r="H31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>148</v>
-      </c>
-      <c r="B32" s="1">
-        <v>2</v>
+        <v>150</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>149</v>
-      </c>
-      <c r="D32" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="E32" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F32" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" t="s">
         <v>135</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>136</v>
-      </c>
-      <c r="H32" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>151</v>
-      </c>
-      <c r="B33" s="1">
+        <v>153</v>
+      </c>
+      <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
-      </c>
-      <c r="D33" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="E33" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F33" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" t="s">
         <v>135</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>136</v>
-      </c>
-      <c r="H33" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>154</v>
-      </c>
-      <c r="B34" s="1">
-        <v>1</v>
+        <v>156</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
-      </c>
-      <c r="D34" t="s">
-        <v>26</v>
+        <v>145</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="E34" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F34" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34" t="s">
         <v>135</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>136</v>
-      </c>
-      <c r="H34" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>157</v>
-      </c>
-      <c r="B35" s="1">
-        <v>3</v>
+        <v>159</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
-      </c>
-      <c r="D35" t="s">
-        <v>146</v>
+        <v>27</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F35" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" t="s">
         <v>135</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>136</v>
-      </c>
-      <c r="H35" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>160</v>
-      </c>
-      <c r="B36" s="1">
-        <v>2</v>
+        <v>162</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" t="s">
-        <v>162</v>
+        <v>141</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
       </c>
       <c r="F36" t="s">
+        <v>134</v>
+      </c>
+      <c r="G36" t="s">
         <v>135</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>136</v>
-      </c>
-      <c r="H36" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>163</v>
-      </c>
-      <c r="B37" s="1">
-        <v>6</v>
-      </c>
-      <c r="C37">
-        <v>100</v>
-      </c>
-      <c r="D37" t="s">
-        <v>142</v>
+        <v>164</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="E37" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F37" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" t="s">
         <v>135</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>136</v>
-      </c>
-      <c r="H37" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>165</v>
-      </c>
-      <c r="B38" s="1">
-        <v>4</v>
+        <v>167</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>166</v>
-      </c>
-      <c r="D38" t="s">
-        <v>146</v>
+        <v>170</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="E38" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G38" t="s">
+        <v>169</v>
+      </c>
+      <c r="H38" t="s">
         <v>136</v>
-      </c>
-      <c r="H38" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>168</v>
-      </c>
-      <c r="B39" s="1">
-        <v>6</v>
+        <v>172</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>169</v>
-      </c>
-      <c r="D39" t="s">
-        <v>171</v>
+        <v>141</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="E39" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F39" t="s">
+        <v>134</v>
+      </c>
+      <c r="G39" t="s">
         <v>135</v>
       </c>
-      <c r="G39" t="s">
-        <v>170</v>
-      </c>
       <c r="H39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>173</v>
-      </c>
-      <c r="B40" s="1">
-        <v>8</v>
+        <v>175</v>
+      </c>
+      <c r="B40">
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>174</v>
-      </c>
-      <c r="D40" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F40" t="s">
+        <v>134</v>
+      </c>
+      <c r="G40" t="s">
         <v>135</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>136</v>
-      </c>
-      <c r="H40" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>176</v>
-      </c>
-      <c r="B41" s="1">
-        <v>16</v>
+        <v>178</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>177</v>
-      </c>
-      <c r="D41" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" t="s">
-        <v>178</v>
+        <v>145</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41">
+        <v>560</v>
       </c>
       <c r="F41" t="s">
+        <v>134</v>
+      </c>
+      <c r="G41" t="s">
         <v>135</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>136</v>
-      </c>
-      <c r="H41" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>179</v>
-      </c>
-      <c r="B42" s="1">
+        <v>180</v>
+      </c>
+      <c r="B42">
         <v>4</v>
       </c>
-      <c r="C42">
-        <v>560</v>
-      </c>
-      <c r="D42" t="s">
-        <v>146</v>
+      <c r="C42" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="E42" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F42" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" t="s">
         <v>135</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>136</v>
-      </c>
-      <c r="H42" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>181</v>
-      </c>
-      <c r="B43" s="1">
+        <v>183</v>
+      </c>
+      <c r="B43">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>182</v>
-      </c>
-      <c r="D43" t="s">
-        <v>142</v>
-      </c>
-      <c r="E43" t="s">
-        <v>183</v>
+        <v>27</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E43">
+        <v>220</v>
       </c>
       <c r="F43" t="s">
+        <v>134</v>
+      </c>
+      <c r="G43" t="s">
         <v>135</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>136</v>
-      </c>
-      <c r="H43" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>184</v>
-      </c>
-      <c r="B44" s="1">
+        <v>185</v>
+      </c>
+      <c r="B44">
         <v>4</v>
       </c>
-      <c r="C44">
-        <v>220</v>
-      </c>
-      <c r="D44" t="s">
-        <v>26</v>
+      <c r="C44" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="E44" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G44" t="s">
+        <v>187</v>
+      </c>
+      <c r="H44" t="s">
         <v>136</v>
-      </c>
-      <c r="H44" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>186</v>
-      </c>
-      <c r="B45" s="1">
-        <v>4</v>
+        <v>189</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>187</v>
-      </c>
-      <c r="D45" t="s">
-        <v>146</v>
-      </c>
-      <c r="E45" t="s">
-        <v>189</v>
+        <v>27</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E45">
+        <v>10</v>
       </c>
       <c r="F45" t="s">
+        <v>134</v>
+      </c>
+      <c r="G45" t="s">
         <v>135</v>
       </c>
-      <c r="G45" t="s">
-        <v>188</v>
-      </c>
       <c r="H45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>190</v>
-      </c>
-      <c r="B46" s="1">
-        <v>3</v>
-      </c>
-      <c r="C46">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s">
-        <v>26</v>
+        <v>191</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="E46" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F46" t="s">
-        <v>135</v>
+        <v>193</v>
       </c>
       <c r="G46" t="s">
-        <v>136</v>
-      </c>
-      <c r="H46" t="s">
-        <v>137</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>192</v>
-      </c>
-      <c r="B47" s="1">
-        <v>6</v>
+        <v>197</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>193</v>
+        <v>200</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E47" t="s">
+        <v>198</v>
       </c>
       <c r="F47" t="s">
+        <v>198</v>
+      </c>
+      <c r="G47" t="s">
         <v>194</v>
       </c>
-      <c r="G47" t="s">
-        <v>195</v>
-      </c>
       <c r="H47" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>197</v>
-      </c>
-      <c r="B48" s="1">
-        <v>2</v>
-      </c>
-      <c r="C48">
-        <v>5002</v>
-      </c>
-      <c r="D48" t="s">
-        <v>200</v>
-      </c>
-      <c r="E48">
-        <v>5002</v>
-      </c>
-      <c r="F48">
-        <v>5002</v>
+        <v>202</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>206</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E48" t="s">
+        <v>203</v>
+      </c>
+      <c r="F48" t="s">
+        <v>203</v>
       </c>
       <c r="G48" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="H48" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>201</v>
-      </c>
-      <c r="B49" s="1">
-        <v>2</v>
-      </c>
-      <c r="C49">
-        <v>5000</v>
-      </c>
-      <c r="D49" t="s">
-        <v>200</v>
-      </c>
-      <c r="E49">
-        <v>5000</v>
-      </c>
-      <c r="F49">
-        <v>5000</v>
+        <v>208</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>211</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E49" t="s">
+        <v>209</v>
+      </c>
+      <c r="F49" t="s">
+        <v>209</v>
       </c>
       <c r="G49" t="s">
-        <v>198</v>
-      </c>
-      <c r="H49" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>203</v>
-      </c>
-      <c r="B50" s="1">
-        <v>2</v>
-      </c>
-      <c r="C50">
-        <v>5001</v>
-      </c>
-      <c r="D50" t="s">
+        <v>212</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
         <v>200</v>
       </c>
-      <c r="E50">
-        <v>5001</v>
-      </c>
-      <c r="F50">
-        <v>5001</v>
+      <c r="D50" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E50" t="s">
+        <v>213</v>
+      </c>
+      <c r="F50" t="s">
+        <v>213</v>
       </c>
       <c r="G50" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="H50" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>205</v>
-      </c>
-      <c r="B51" s="1">
-        <v>1</v>
+        <v>217</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
-      </c>
-      <c r="D51" t="s">
-        <v>209</v>
+        <v>56</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="E51" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F51" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="G51" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>211</v>
-      </c>
-      <c r="B52" s="1">
-        <v>2</v>
+        <v>220</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>212</v>
-      </c>
-      <c r="D52" t="s">
-        <v>214</v>
+        <v>225</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="E52" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="F52" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="G52" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="H52" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>216</v>
-      </c>
-      <c r="B53" s="1">
-        <v>1</v>
+        <v>227</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>217</v>
-      </c>
-      <c r="D53" t="s">
-        <v>220</v>
+        <v>231</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E53" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="F53" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="G53" t="s">
-        <v>218</v>
-      </c>
-      <c r="H53" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>222</v>
-      </c>
-      <c r="B54" s="1">
-        <v>1</v>
-      </c>
-      <c r="C54" t="s">
-        <v>223</v>
-      </c>
-      <c r="D54" t="s">
-        <v>225</v>
-      </c>
-      <c r="E54" t="s">
-        <v>223</v>
-      </c>
-      <c r="F54" t="s">
-        <v>223</v>
-      </c>
-      <c r="G54" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>226</v>
-      </c>
-      <c r="B55" s="1">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
-        <v>227</v>
-      </c>
-      <c r="D55" t="s">
-        <v>214</v>
-      </c>
-      <c r="E55" t="s">
-        <v>230</v>
-      </c>
-      <c r="F55" t="s">
-        <v>227</v>
-      </c>
-      <c r="G55" t="s">
-        <v>228</v>
-      </c>
-      <c r="H55" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>231</v>
-      </c>
-      <c r="B56" s="1">
-        <v>2</v>
-      </c>
-      <c r="C56" t="s">
-        <v>232</v>
-      </c>
-      <c r="D56" t="s">
-        <v>57</v>
-      </c>
-      <c r="E56" t="s">
-        <v>232</v>
-      </c>
-      <c r="F56" t="s">
-        <v>232</v>
-      </c>
-      <c r="G56" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>234</v>
-      </c>
-      <c r="B57" s="1">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
-        <v>235</v>
-      </c>
-      <c r="F57" t="s">
-        <v>236</v>
-      </c>
-      <c r="G57" t="s">
-        <v>237</v>
-      </c>
-      <c r="H57" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>239</v>
-      </c>
-      <c r="B58" s="1">
-        <v>2</v>
-      </c>
-      <c r="C58" t="s">
-        <v>240</v>
-      </c>
-      <c r="F58" t="s">
-        <v>241</v>
-      </c>
-      <c r="G58" t="s">
-        <v>237</v>
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3 D4:D10" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>